<commit_message>
new plot first year
</commit_message>
<xml_diff>
--- a/Model/output/midresults.xlsx
+++ b/Model/output/midresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Studie TUD\Msc\Year 6\Q2 Subsurface storage for energy, water and climate\Project\design-ASR-CEGM2006\Model\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E8F03B-D388-4E54-8273-F8EE7BFE6661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD43C1E3-7440-4466-9463-6C3DAF5B0094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7055,13 +7055,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7482,9 +7482,9 @@
       <selection activeCell="E315" sqref="E315"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.5">
+    <row r="1" spans="1:1" ht="30">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -9710,9 +9710,9 @@
       <selection sqref="A1:A117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.5">
+    <row r="1" spans="1:1" ht="30">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>

</xml_diff>